<commit_message>
Brass QC - Scan Btn using Scanner - Row Highlight without modalpopup and and anotehr row to swap on interaction - Fixed
</commit_message>
<xml_diff>
--- a/Doc/Barcode.xlsx
+++ b/Doc/Barcode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Workspace\Watchcase\TTT-Jan2026\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0652262-2F51-4C04-8A40-7CC298FB6BBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9765031F-442D-4180-A059-0490A9BF8957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{1897626A-E385-4393-931F-CA99E7C3BE4B}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="151">
   <si>
     <t>JB-A00001</t>
   </si>
@@ -387,13 +387,106 @@
   </si>
   <si>
     <t>NB-A00025</t>
+  </si>
+  <si>
+    <t>NB-A00051</t>
+  </si>
+  <si>
+    <t>NB-A00052</t>
+  </si>
+  <si>
+    <t>NB-A00053</t>
+  </si>
+  <si>
+    <t>NB-A00054</t>
+  </si>
+  <si>
+    <t>NB-A00055</t>
+  </si>
+  <si>
+    <t>NB-A00056</t>
+  </si>
+  <si>
+    <t>NB-A00057</t>
+  </si>
+  <si>
+    <t>NB-A00058</t>
+  </si>
+  <si>
+    <t>NB-A00059</t>
+  </si>
+  <si>
+    <t>NB-A00060</t>
+  </si>
+  <si>
+    <t>NB-A00061</t>
+  </si>
+  <si>
+    <t>NB-A00062</t>
+  </si>
+  <si>
+    <t>NB-A00063</t>
+  </si>
+  <si>
+    <t>NB-A00064</t>
+  </si>
+  <si>
+    <t>NB-A00065</t>
+  </si>
+  <si>
+    <t>NB-A00066</t>
+  </si>
+  <si>
+    <t>NB-A00067</t>
+  </si>
+  <si>
+    <t>NB-A00068</t>
+  </si>
+  <si>
+    <t>NB-A00069</t>
+  </si>
+  <si>
+    <t>NB-A00070</t>
+  </si>
+  <si>
+    <t>NB-A00071</t>
+  </si>
+  <si>
+    <t>NB-A00072</t>
+  </si>
+  <si>
+    <t>NB-A00073</t>
+  </si>
+  <si>
+    <t>NB-A00074</t>
+  </si>
+  <si>
+    <t>NB-A00075</t>
+  </si>
+  <si>
+    <t>NB-A00026</t>
+  </si>
+  <si>
+    <t>NB-A00027</t>
+  </si>
+  <si>
+    <t>NB-A00028</t>
+  </si>
+  <si>
+    <t>NB-A00029</t>
+  </si>
+  <si>
+    <t>NB-A00030</t>
+  </si>
+  <si>
+    <t>NB-A00031</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -419,6 +512,19 @@
       <name val="IDAutomationHC39M Free Version"/>
       <family val="1"/>
       <charset val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -447,7 +553,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -457,6 +563,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1402,58 +1515,58 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3C6EDE2-EEAC-4F28-8427-6EDF59F4B7EE}">
   <dimension ref="B3:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.7265625" style="1"/>
-    <col min="2" max="2" width="0.6328125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="3.26953125" style="7" customWidth="1"/>
     <col min="3" max="3" width="29.81640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="0.81640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="3.453125" style="6" customWidth="1"/>
     <col min="5" max="5" width="30.36328125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="0.453125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="4" style="6" customWidth="1"/>
     <col min="7" max="7" width="23.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.6328125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="0.453125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="1.6328125" style="6" customWidth="1"/>
     <col min="10" max="10" width="23.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.7265625" style="1"/>
-    <col min="12" max="12" width="0.26953125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="3.26953125" style="6" customWidth="1"/>
     <col min="13" max="13" width="23.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:13" ht="64.5" x14ac:dyDescent="0.35">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>95</v>
       </c>
       <c r="C3" s="4" t="str">
         <f>"*" &amp; B3 &amp; "*"</f>
         <v>*NB-A00001*</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="5" t="s">
         <v>100</v>
       </c>
       <c r="E3" s="4" t="str">
         <f>"*" &amp; D3 &amp; "*"</f>
         <v>*NB-A00006*</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="5" t="s">
         <v>105</v>
       </c>
       <c r="G3" s="4" t="str">
         <f>"*" &amp; F3 &amp; "*"</f>
         <v>*NB-A00011*</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="5" t="s">
         <v>110</v>
       </c>
       <c r="J3" s="4" t="str">
         <f>"*" &amp; I3 &amp; "*"</f>
         <v>*NB-A00016*</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L3" s="5" t="s">
         <v>115</v>
       </c>
       <c r="M3" s="4" t="str">
@@ -1462,35 +1575,35 @@
       </c>
     </row>
     <row r="4" spans="2:13" ht="64.5" x14ac:dyDescent="0.35">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="5" t="s">
         <v>96</v>
       </c>
       <c r="C4" s="4" t="str">
         <f>"*" &amp; B4 &amp; "*"</f>
         <v>*NB-A00002*</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="5" t="s">
         <v>101</v>
       </c>
       <c r="E4" s="4" t="str">
         <f>"*" &amp; D4 &amp; "*"</f>
         <v>*NB-A00007*</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="5" t="s">
         <v>106</v>
       </c>
       <c r="G4" s="4" t="str">
         <f>"*" &amp; F4 &amp; "*"</f>
         <v>*NB-A00012*</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="5" t="s">
         <v>111</v>
       </c>
       <c r="J4" s="4" t="str">
         <f t="shared" ref="J4:J7" si="0">"*" &amp; I4 &amp; "*"</f>
         <v>*NB-A00017*</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="5" t="s">
         <v>116</v>
       </c>
       <c r="M4" s="4" t="str">
@@ -1499,35 +1612,35 @@
       </c>
     </row>
     <row r="5" spans="2:13" ht="64.5" x14ac:dyDescent="0.35">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="5" t="s">
         <v>97</v>
       </c>
       <c r="C5" s="4" t="str">
         <f>"*" &amp; B5 &amp; "*"</f>
         <v>*NB-A00003*</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="5" t="s">
         <v>102</v>
       </c>
       <c r="E5" s="4" t="str">
         <f>"*" &amp; D5 &amp; "*"</f>
         <v>*NB-A00008*</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="5" t="s">
         <v>107</v>
       </c>
       <c r="G5" s="4" t="str">
         <f>"*" &amp; F5 &amp; "*"</f>
         <v>*NB-A00013*</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="5" t="s">
         <v>112</v>
       </c>
       <c r="J5" s="4" t="str">
         <f t="shared" si="0"/>
         <v>*NB-A00018*</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L5" s="5" t="s">
         <v>117</v>
       </c>
       <c r="M5" s="4" t="str">
@@ -1536,35 +1649,35 @@
       </c>
     </row>
     <row r="6" spans="2:13" ht="64.5" x14ac:dyDescent="0.35">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="5" t="s">
         <v>98</v>
       </c>
       <c r="C6" s="4" t="str">
         <f t="shared" ref="C6:C7" si="2">"*" &amp; B6 &amp; "*"</f>
         <v>*NB-A00004*</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="5" t="s">
         <v>103</v>
       </c>
       <c r="E6" s="4" t="str">
         <f>"*" &amp; D6 &amp; "*"</f>
         <v>*NB-A00009*</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="5" t="s">
         <v>108</v>
       </c>
       <c r="G6" s="4" t="str">
         <f>"*" &amp; F6 &amp; "*"</f>
         <v>*NB-A00014*</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6" s="5" t="s">
         <v>113</v>
       </c>
       <c r="J6" s="4" t="str">
         <f t="shared" si="0"/>
         <v>*NB-A00019*</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="L6" s="5" t="s">
         <v>118</v>
       </c>
       <c r="M6" s="4" t="str">
@@ -1573,35 +1686,35 @@
       </c>
     </row>
     <row r="7" spans="2:13" ht="64.5" x14ac:dyDescent="0.35">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="5" t="s">
         <v>99</v>
       </c>
       <c r="C7" s="4" t="str">
         <f t="shared" si="2"/>
         <v>*NB-A00005*</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="5" t="s">
         <v>104</v>
       </c>
       <c r="E7" s="4" t="str">
         <f>"*" &amp; D7 &amp; "*"</f>
         <v>*NB-A00010*</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="5" t="s">
         <v>109</v>
       </c>
       <c r="G7" s="4" t="str">
         <f>"*" &amp; F7 &amp; "*"</f>
         <v>*NB-A00015*</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="5" t="s">
         <v>114</v>
       </c>
       <c r="J7" s="4" t="str">
         <f t="shared" si="0"/>
         <v>*NB-A00020*</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="L7" s="5" t="s">
         <v>119</v>
       </c>
       <c r="M7" s="4" t="str">
@@ -1610,35 +1723,35 @@
       </c>
     </row>
     <row r="9" spans="2:13" ht="64.5" x14ac:dyDescent="0.35">
-      <c r="B9" s="2" t="s">
-        <v>25</v>
+      <c r="B9" s="5" t="s">
+        <v>145</v>
       </c>
       <c r="C9" s="4" t="str">
         <f>"*" &amp; B9 &amp; "*"</f>
-        <v>*JB-A00026*</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>30</v>
+        <v>*NB-A00026*</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>150</v>
       </c>
       <c r="E9" s="4" t="str">
         <f>"*" &amp; D9 &amp; "*"</f>
-        <v>*JB-A00031*</v>
-      </c>
-      <c r="F9" s="2" t="s">
+        <v>*NB-A00031*</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>35</v>
       </c>
       <c r="G9" s="4" t="str">
         <f>"*" &amp; F9 &amp; "*"</f>
         <v>*JB-A00036*</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="5" t="s">
         <v>40</v>
       </c>
       <c r="J9" s="4" t="str">
         <f>"*" &amp; I9 &amp; "*"</f>
         <v>*JB-A00041*</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="L9" s="5" t="s">
         <v>45</v>
       </c>
       <c r="M9" s="4" t="str">
@@ -1647,35 +1760,35 @@
       </c>
     </row>
     <row r="10" spans="2:13" ht="64.5" x14ac:dyDescent="0.35">
-      <c r="B10" s="2" t="s">
-        <v>26</v>
+      <c r="B10" s="5" t="s">
+        <v>146</v>
       </c>
       <c r="C10" s="4" t="str">
         <f t="shared" ref="C10:C22" si="4">"*" &amp; B10 &amp; "*"</f>
-        <v>*JB-A00027*</v>
-      </c>
-      <c r="D10" s="2" t="s">
+        <v>*NB-A00027*</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>31</v>
       </c>
       <c r="E10" s="4" t="str">
         <f>"*" &amp; D10 &amp; "*"</f>
         <v>*JB-A00032*</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="5" t="s">
         <v>36</v>
       </c>
       <c r="G10" s="4" t="str">
         <f>"*" &amp; F10 &amp; "*"</f>
         <v>*JB-A00037*</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="I10" s="5" t="s">
         <v>41</v>
       </c>
       <c r="J10" s="4" t="str">
         <f t="shared" ref="J10:J13" si="5">"*" &amp; I10 &amp; "*"</f>
         <v>*JB-A00042*</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="L10" s="5" t="s">
         <v>46</v>
       </c>
       <c r="M10" s="4" t="str">
@@ -1684,35 +1797,35 @@
       </c>
     </row>
     <row r="11" spans="2:13" ht="64.5" x14ac:dyDescent="0.35">
-      <c r="B11" s="2" t="s">
-        <v>27</v>
+      <c r="B11" s="5" t="s">
+        <v>147</v>
       </c>
       <c r="C11" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>*JB-A00028*</v>
-      </c>
-      <c r="D11" s="2" t="s">
+        <v>*NB-A00028*</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>32</v>
       </c>
       <c r="E11" s="4" t="str">
         <f>"*" &amp; D11 &amp; "*"</f>
         <v>*JB-A00033*</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="5" t="s">
         <v>37</v>
       </c>
       <c r="G11" s="4" t="str">
         <f>"*" &amp; F11 &amp; "*"</f>
         <v>*JB-A00038*</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="5" t="s">
         <v>42</v>
       </c>
       <c r="J11" s="4" t="str">
         <f t="shared" si="5"/>
         <v>*JB-A00043*</v>
       </c>
-      <c r="L11" s="2" t="s">
+      <c r="L11" s="5" t="s">
         <v>47</v>
       </c>
       <c r="M11" s="4" t="str">
@@ -1721,35 +1834,35 @@
       </c>
     </row>
     <row r="12" spans="2:13" ht="64.5" x14ac:dyDescent="0.35">
-      <c r="B12" s="2" t="s">
-        <v>28</v>
+      <c r="B12" s="5" t="s">
+        <v>148</v>
       </c>
       <c r="C12" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>*JB-A00029*</v>
-      </c>
-      <c r="D12" s="2" t="s">
+        <v>*NB-A00029*</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>33</v>
       </c>
       <c r="E12" s="4" t="str">
         <f>"*" &amp; D12 &amp; "*"</f>
         <v>*JB-A00034*</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="5" t="s">
         <v>38</v>
       </c>
       <c r="G12" s="4" t="str">
         <f>"*" &amp; F12 &amp; "*"</f>
         <v>*JB-A00039*</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="I12" s="5" t="s">
         <v>43</v>
       </c>
       <c r="J12" s="4" t="str">
         <f t="shared" si="5"/>
         <v>*JB-A00044*</v>
       </c>
-      <c r="L12" s="2" t="s">
+      <c r="L12" s="5" t="s">
         <v>48</v>
       </c>
       <c r="M12" s="4" t="str">
@@ -1758,35 +1871,35 @@
       </c>
     </row>
     <row r="13" spans="2:13" ht="64.5" x14ac:dyDescent="0.35">
-      <c r="B13" s="2" t="s">
-        <v>29</v>
+      <c r="B13" s="5" t="s">
+        <v>149</v>
       </c>
       <c r="C13" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>*JB-A00030*</v>
-      </c>
-      <c r="D13" s="2" t="s">
+        <v>*NB-A00030*</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>34</v>
       </c>
       <c r="E13" s="4" t="str">
         <f>"*" &amp; D13 &amp; "*"</f>
         <v>*JB-A00035*</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="5" t="s">
         <v>39</v>
       </c>
       <c r="G13" s="4" t="str">
         <f>"*" &amp; F13 &amp; "*"</f>
         <v>*JB-A00040*</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" s="5" t="s">
         <v>44</v>
       </c>
       <c r="J13" s="4" t="str">
         <f t="shared" si="5"/>
         <v>*JB-A00045*</v>
       </c>
-      <c r="L13" s="2" t="s">
+      <c r="L13" s="5" t="s">
         <v>49</v>
       </c>
       <c r="M13" s="4" t="str">
@@ -1795,228 +1908,228 @@
       </c>
     </row>
     <row r="18" spans="2:13" ht="64.5" x14ac:dyDescent="0.35">
-      <c r="B18" s="2" t="s">
-        <v>50</v>
+      <c r="B18" s="5" t="s">
+        <v>120</v>
       </c>
       <c r="C18" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>*JB-A00051*</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>55</v>
+        <v>*NB-A00051*</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>125</v>
       </c>
       <c r="E18" s="4" t="str">
         <f>"*" &amp; D18 &amp; "*"</f>
-        <v>*JB-A00056*</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>60</v>
+        <v>*NB-A00056*</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>130</v>
       </c>
       <c r="G18" s="4" t="str">
         <f>"*" &amp; F18 &amp; "*"</f>
-        <v>*JB-A00061*</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>65</v>
+        <v>*NB-A00061*</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>135</v>
       </c>
       <c r="J18" s="4" t="str">
         <f>"*" &amp; I18 &amp; "*"</f>
-        <v>*JB-A00066*</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>70</v>
+        <v>*NB-A00066*</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>140</v>
       </c>
       <c r="M18" s="4" t="str">
         <f>"*" &amp; L18 &amp; "*"</f>
-        <v>*JB-A00071*</v>
+        <v>*NB-A00071*</v>
       </c>
     </row>
     <row r="19" spans="2:13" ht="64.5" x14ac:dyDescent="0.35">
-      <c r="B19" s="2" t="s">
-        <v>51</v>
+      <c r="B19" s="5" t="s">
+        <v>121</v>
       </c>
       <c r="C19" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>*JB-A00052*</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>56</v>
+        <v>*NB-A00052*</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>126</v>
       </c>
       <c r="E19" s="4" t="str">
         <f>"*" &amp; D19 &amp; "*"</f>
-        <v>*JB-A00057*</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>61</v>
+        <v>*NB-A00057*</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="G19" s="4" t="str">
         <f>"*" &amp; F19 &amp; "*"</f>
-        <v>*JB-A00062*</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>66</v>
+        <v>*NB-A00062*</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>136</v>
       </c>
       <c r="J19" s="4" t="str">
         <f t="shared" ref="J19:J22" si="6">"*" &amp; I19 &amp; "*"</f>
-        <v>*JB-A00067*</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>71</v>
+        <v>*NB-A00067*</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>141</v>
       </c>
       <c r="M19" s="4" t="str">
         <f t="shared" ref="M19:M22" si="7">"*" &amp; L19 &amp; "*"</f>
-        <v>*JB-A00072*</v>
+        <v>*NB-A00072*</v>
       </c>
     </row>
     <row r="20" spans="2:13" ht="64.5" x14ac:dyDescent="0.35">
-      <c r="B20" s="2" t="s">
-        <v>52</v>
+      <c r="B20" s="5" t="s">
+        <v>122</v>
       </c>
       <c r="C20" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>*JB-A00053*</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>57</v>
+        <v>*NB-A00053*</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>127</v>
       </c>
       <c r="E20" s="4" t="str">
         <f>"*" &amp; D20 &amp; "*"</f>
-        <v>*JB-A00058*</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>62</v>
+        <v>*NB-A00058*</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>132</v>
       </c>
       <c r="G20" s="4" t="str">
         <f>"*" &amp; F20 &amp; "*"</f>
-        <v>*JB-A00063*</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>67</v>
+        <v>*NB-A00063*</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>137</v>
       </c>
       <c r="J20" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>*JB-A00068*</v>
-      </c>
-      <c r="L20" s="2" t="s">
-        <v>72</v>
+        <v>*NB-A00068*</v>
+      </c>
+      <c r="L20" s="5" t="s">
+        <v>142</v>
       </c>
       <c r="M20" s="4" t="str">
         <f t="shared" si="7"/>
-        <v>*JB-A00073*</v>
+        <v>*NB-A00073*</v>
       </c>
     </row>
     <row r="21" spans="2:13" ht="64.5" x14ac:dyDescent="0.35">
-      <c r="B21" s="2" t="s">
-        <v>53</v>
+      <c r="B21" s="5" t="s">
+        <v>123</v>
       </c>
       <c r="C21" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>*JB-A00054*</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>58</v>
+        <v>*NB-A00054*</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>128</v>
       </c>
       <c r="E21" s="4" t="str">
         <f>"*" &amp; D21 &amp; "*"</f>
-        <v>*JB-A00059*</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>63</v>
+        <v>*NB-A00059*</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>133</v>
       </c>
       <c r="G21" s="4" t="str">
         <f>"*" &amp; F21 &amp; "*"</f>
-        <v>*JB-A00064*</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>68</v>
+        <v>*NB-A00064*</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>138</v>
       </c>
       <c r="J21" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>*JB-A00069*</v>
-      </c>
-      <c r="L21" s="2" t="s">
-        <v>73</v>
+        <v>*NB-A00069*</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>143</v>
       </c>
       <c r="M21" s="4" t="str">
         <f t="shared" si="7"/>
-        <v>*JB-A00074*</v>
+        <v>*NB-A00074*</v>
       </c>
     </row>
     <row r="22" spans="2:13" ht="64.5" x14ac:dyDescent="0.35">
-      <c r="B22" s="2" t="s">
-        <v>54</v>
+      <c r="B22" s="5" t="s">
+        <v>124</v>
       </c>
       <c r="C22" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>*JB-A00055*</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>59</v>
+        <v>*NB-A00055*</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>129</v>
       </c>
       <c r="E22" s="4" t="str">
         <f>"*" &amp; D22 &amp; "*"</f>
-        <v>*JB-A00060*</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>64</v>
+        <v>*NB-A00060*</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>134</v>
       </c>
       <c r="G22" s="4" t="str">
         <f>"*" &amp; F22 &amp; "*"</f>
-        <v>*JB-A00065*</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>69</v>
+        <v>*NB-A00065*</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>139</v>
       </c>
       <c r="J22" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>*JB-A00070*</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>74</v>
+        <v>*NB-A00070*</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>144</v>
       </c>
       <c r="M22" s="4" t="str">
         <f t="shared" si="7"/>
-        <v>*JB-A00075*</v>
+        <v>*NB-A00075*</v>
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B23" s="1"/>
+      <c r="B23" s="6"/>
       <c r="C23" s="1"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B24" s="1"/>
+      <c r="B24" s="6"/>
       <c r="C24" s="1"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B25" s="1"/>
+      <c r="B25" s="6"/>
       <c r="C25" s="1"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B26" s="1"/>
+      <c r="B26" s="6"/>
       <c r="C26" s="1"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B27" s="1"/>
+      <c r="B27" s="6"/>
       <c r="C27" s="1"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B28" s="1"/>
+      <c r="B28" s="6"/>
       <c r="C28" s="1"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B29" s="1"/>
+      <c r="B29" s="6"/>
       <c r="C29" s="1"/>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B30" s="1"/>
+      <c r="B30" s="6"/>
       <c r="C30" s="1"/>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B31" s="1"/>
+      <c r="B31" s="6"/>
       <c r="C31" s="1"/>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B32" s="1"/>
+      <c r="B32" s="6"/>
       <c r="C32" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
IQF - Scan Btn using scanner - Row highlight without modalpopup irrespective of pagination & manual click pointers to func as is - Fixed
</commit_message>
<xml_diff>
--- a/Doc/Barcode.xlsx
+++ b/Doc/Barcode.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Workspace\Watchcase\TTT-Jan2026\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9765031F-442D-4180-A059-0490A9BF8957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC649CB-D54D-4425-BDED-8277134D2BEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{1897626A-E385-4393-931F-CA99E7C3BE4B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{1897626A-E385-4393-931F-CA99E7C3BE4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Jig QR ID" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="175">
   <si>
     <t>JB-A00001</t>
   </si>
@@ -480,6 +480,78 @@
   </si>
   <si>
     <t>NB-A00031</t>
+  </si>
+  <si>
+    <t>JB-A00100</t>
+  </si>
+  <si>
+    <t>JB-A00101</t>
+  </si>
+  <si>
+    <t>JB-A00102</t>
+  </si>
+  <si>
+    <t>JB-A00103</t>
+  </si>
+  <si>
+    <t>JB-A00104</t>
+  </si>
+  <si>
+    <t>JB-A00105</t>
+  </si>
+  <si>
+    <t>JB-A00110</t>
+  </si>
+  <si>
+    <t>JB-A00111</t>
+  </si>
+  <si>
+    <t>JB-A00112</t>
+  </si>
+  <si>
+    <t>JB-A00113</t>
+  </si>
+  <si>
+    <t>JB-A00114</t>
+  </si>
+  <si>
+    <t>JB-A00115</t>
+  </si>
+  <si>
+    <t>JB-A00116</t>
+  </si>
+  <si>
+    <t>JB-A00117</t>
+  </si>
+  <si>
+    <t>JB-A00118</t>
+  </si>
+  <si>
+    <t>JB-A00119</t>
+  </si>
+  <si>
+    <t>JB-A00120</t>
+  </si>
+  <si>
+    <t>JB-A00121</t>
+  </si>
+  <si>
+    <t>JB-A00122</t>
+  </si>
+  <si>
+    <t>JB-A00123</t>
+  </si>
+  <si>
+    <t>JB-A00124</t>
+  </si>
+  <si>
+    <t>JB-A00125</t>
+  </si>
+  <si>
+    <t>JB-A00126</t>
+  </si>
+  <si>
+    <t>JB-A00127</t>
   </si>
 </sst>
 </file>
@@ -1515,7 +1587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3C6EDE2-EEAC-4F28-8427-6EDF59F4B7EE}">
   <dimension ref="B3:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -2143,8 +2215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7419E62F-278C-4ED6-A2AE-608923B5D131}">
   <dimension ref="B3:M32"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2726,32 +2798,188 @@
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-    </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-    </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-    </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
+    <row r="25" spans="2:13" ht="64.5" x14ac:dyDescent="0.35">
+      <c r="B25" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C25" s="4" t="str">
+        <f t="shared" ref="C25" si="8">"*" &amp; B25 &amp; "*"</f>
+        <v>*JB-A00100*</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E25" s="4" t="str">
+        <f t="shared" ref="E25" si="9">"*" &amp; D25 &amp; "*"</f>
+        <v>*JB-A00110*</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G25" s="4" t="str">
+        <f t="shared" ref="G25" si="10">"*" &amp; F25 &amp; "*"</f>
+        <v>*JB-A00116*</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="J25" s="4" t="str">
+        <f t="shared" ref="J25" si="11">"*" &amp; I25 &amp; "*"</f>
+        <v>*JB-A00122*</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" ht="64.5" x14ac:dyDescent="0.35">
+      <c r="B26" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C26" s="4" t="str">
+        <f t="shared" ref="C26:C30" si="12">"*" &amp; B26 &amp; "*"</f>
+        <v>*JB-A00101*</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E26" s="4" t="str">
+        <f t="shared" ref="E26:E30" si="13">"*" &amp; D26 &amp; "*"</f>
+        <v>*JB-A00111*</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="G26" s="4" t="str">
+        <f t="shared" ref="G26:G30" si="14">"*" &amp; F26 &amp; "*"</f>
+        <v>*JB-A00117*</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="J26" s="4" t="str">
+        <f t="shared" ref="J26:J30" si="15">"*" &amp; I26 &amp; "*"</f>
+        <v>*JB-A00123*</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" ht="64.5" x14ac:dyDescent="0.35">
+      <c r="B27" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C27" s="4" t="str">
+        <f t="shared" si="12"/>
+        <v>*JB-A00102*</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E27" s="4" t="str">
+        <f t="shared" si="13"/>
+        <v>*JB-A00112*</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G27" s="4" t="str">
+        <f t="shared" si="14"/>
+        <v>*JB-A00118*</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="J27" s="4" t="str">
+        <f t="shared" si="15"/>
+        <v>*JB-A00124*</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" ht="64.5" x14ac:dyDescent="0.35">
+      <c r="B28" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C28" s="4" t="str">
+        <f t="shared" si="12"/>
+        <v>*JB-A00103*</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E28" s="4" t="str">
+        <f t="shared" si="13"/>
+        <v>*JB-A00113*</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="G28" s="4" t="str">
+        <f t="shared" si="14"/>
+        <v>*JB-A00119*</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="J28" s="4" t="str">
+        <f t="shared" si="15"/>
+        <v>*JB-A00125*</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" ht="64.5" x14ac:dyDescent="0.35">
+      <c r="B29" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C29" s="4" t="str">
+        <f t="shared" si="12"/>
+        <v>*JB-A00104*</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E29" s="4" t="str">
+        <f t="shared" si="13"/>
+        <v>*JB-A00114*</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G29" s="4" t="str">
+        <f t="shared" si="14"/>
+        <v>*JB-A00120*</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="J29" s="4" t="str">
+        <f t="shared" si="15"/>
+        <v>*JB-A00126*</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" ht="64.5" x14ac:dyDescent="0.35">
+      <c r="B30" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C30" s="4" t="str">
+        <f t="shared" si="12"/>
+        <v>*JB-A00105*</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E30" s="4" t="str">
+        <f t="shared" si="13"/>
+        <v>*JB-A00115*</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="G30" s="4" t="str">
+        <f t="shared" si="14"/>
+        <v>*JB-A00121*</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="J30" s="4" t="str">
+        <f t="shared" si="15"/>
+        <v>*JB-A00127*</v>
+      </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B31" s="1"/>
+      <c r="B31" s="2"/>
       <c r="C31" s="1"/>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.35">

</xml_diff>